<commit_message>
run tagseq w/ HISAT2
</commit_message>
<xml_diff>
--- a/202107_EXP2/desiccation/20210713_EXP2/tank_temps.xlsx
+++ b/202107_EXP2/desiccation/20210713_EXP2/tank_temps.xlsx
@@ -1,27 +1,37 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24131"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25427"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattg\Dropbox\UW\Postdoc\[2021] NOPP_gigas_ploidy_temp\NOPP-cgigas-ploidy-temp\202107_EX2\desiccation\20210713_EXP2\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mattg\Dropbox\UW\Postdoc\2021_NOPP_gigas_ploidy_temp\NOPP-gigas-ploidy-temp\202107_EXP2\desiccation\20210713_EXP2\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E459CB93-BA70-463B-81A8-9525396BAC74}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C273C2E-A204-471E-8DBD-3512658E08AD}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-103" yWindow="-103" windowWidth="33120" windowHeight="18120" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="data" sheetId="2" r:id="rId1"/>
     <sheet name="combo" sheetId="3" r:id="rId2"/>
   </sheets>
-  <calcPr calcId="181029"/>
+  <calcPr calcId="191029"/>
+  <extLst>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+        <xcalcf:feature name="microsoft.com:LET_WF"/>
+        <xcalcf:feature name="microsoft.com:LAMBDA_WF"/>
+      </xcalcf:calcFeatures>
+    </ext>
+  </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="83" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="84" uniqueCount="18">
   <si>
     <t>tank_A</t>
   </si>
@@ -72,6 +82,9 @@
   </si>
   <si>
     <t>oysters</t>
+  </si>
+  <si>
+    <t>hour</t>
   </si>
 </sst>
 </file>
@@ -940,23 +953,23 @@
       <selection pane="bottomLeft" activeCell="Q18" sqref="Q18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.4609375" style="1" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="6.765625" style="1" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="6.69140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="6.61328125" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="6.765625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="10.921875" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="11.84375" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="6.53515625" style="1" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="6.61328125" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="6.3828125" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="6.61328125" bestFit="1" customWidth="1"/>
-    <col min="12" max="13" width="11.84375" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="14.42578125" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.7109375" style="1" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="6.7109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="10.85546875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="11.85546875" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="6.5703125" style="1" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="6.42578125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="6.5703125" bestFit="1" customWidth="1"/>
+    <col min="12" max="13" width="11.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="3" t="s">
         <v>12</v>
       </c>
@@ -997,7 +1010,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="2">
         <v>44390.291666666664</v>
       </c>
@@ -1042,7 +1055,7 @@
         <v>0.86120071218425553</v>
       </c>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="2">
         <v>44390.302083333336</v>
       </c>
@@ -1087,7 +1100,7 @@
         <v>0.86542378828718147</v>
       </c>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A4" s="2">
         <v>44390.3125</v>
       </c>
@@ -1132,7 +1145,7 @@
         <v>0.91230020643791643</v>
       </c>
     </row>
-    <row r="5" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A5" s="2">
         <v>44390.322916666664</v>
       </c>
@@ -1177,7 +1190,7 @@
         <v>0.83802844024929568</v>
       </c>
     </row>
-    <row r="6" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A6" s="2">
         <v>44390.333333333336</v>
       </c>
@@ -1222,7 +1235,7 @@
         <v>0.86446033261605748</v>
       </c>
     </row>
-    <row r="7" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A7" s="2">
         <v>44390.34375</v>
       </c>
@@ -1267,7 +1280,7 @@
         <v>3.4030623463776473</v>
       </c>
     </row>
-    <row r="8" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A8" s="2">
         <v>44390.354166666664</v>
       </c>
@@ -1312,7 +1325,7 @@
         <v>1.913711489923877</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A9" s="2">
         <v>44390.364583333336</v>
       </c>
@@ -1357,7 +1370,7 @@
         <v>1.7094711657897794</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A10" s="2">
         <v>44390.375</v>
       </c>
@@ -1402,7 +1415,7 @@
         <v>2.8714108030722136</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A11" s="2">
         <v>44390.385416666664</v>
       </c>
@@ -1447,7 +1460,7 @@
         <v>1.3859413166989918</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A12" s="2">
         <v>44390.395833333336</v>
       </c>
@@ -1492,7 +1505,7 @@
         <v>1.1925987031129408</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A13" s="2">
         <v>44390.40625</v>
       </c>
@@ -1537,7 +1550,7 @@
         <v>1.7726510278863876</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A14" s="2">
         <v>44390.416666666664</v>
       </c>
@@ -1582,7 +1595,7 @@
         <v>1.9859401635833147</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A15" s="2">
         <v>44390.427083333336</v>
       </c>
@@ -1627,7 +1640,7 @@
         <v>2.8943911276812568</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A16" s="2">
         <v>44390.4375</v>
       </c>
@@ -1672,7 +1685,7 @@
         <v>4.7325776979006626</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A17" s="2">
         <v>44390.447916666664</v>
       </c>
@@ -1717,7 +1730,7 @@
         <v>4.8722000506273737</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A18" s="2">
         <v>44390.458333333336</v>
       </c>
@@ -1762,7 +1775,7 @@
         <v>5.1097129730217432</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A19" s="2">
         <v>44390.46875</v>
       </c>
@@ -1807,7 +1820,7 @@
         <v>5.6402386178836998</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A20" s="2">
         <v>44390.479166666664</v>
       </c>
@@ -1852,7 +1865,7 @@
         <v>5.1371806470086367</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A21" s="2">
         <v>44390.489583333336</v>
       </c>
@@ -1897,7 +1910,7 @@
         <v>5.2028037313228275</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A22" s="2">
         <v>44390.5</v>
       </c>
@@ -1942,7 +1955,7 @@
         <v>4.9068829209590916</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A23" s="2">
         <v>44390.510416666664</v>
       </c>
@@ -1987,7 +2000,7 @@
         <v>2.2928784674872489</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A24" s="2">
         <v>44390.520833333336</v>
       </c>
@@ -2032,7 +2045,7 @@
         <v>2.5124274450552124</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A25" s="2">
         <v>44390.53125</v>
       </c>
@@ -2077,7 +2090,7 @@
         <v>2.8848382392548189</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A26" s="2">
         <v>44390.541666666664</v>
       </c>
@@ -2122,7 +2135,7 @@
         <v>3.8432570822155565</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A27" s="2">
         <v>44390.552083333336</v>
       </c>
@@ -2167,7 +2180,7 @@
         <v>4.4639995146355647</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A28" s="2">
         <v>44390.5625</v>
       </c>
@@ -2212,7 +2225,7 @@
         <v>3.9437714605860639</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A29" s="2">
         <v>44390.572916666664</v>
       </c>
@@ -2257,373 +2270,373 @@
         <v>4.0146346865769633</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A30" s="2"/>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A31" s="2"/>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A32" s="2"/>
     </row>
-    <row r="33" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A33" s="2"/>
     </row>
-    <row r="34" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A34" s="2"/>
     </row>
-    <row r="35" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A35" s="2"/>
     </row>
-    <row r="36" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A36" s="2"/>
     </row>
-    <row r="37" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A37" s="2"/>
     </row>
-    <row r="38" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A38" s="2"/>
     </row>
-    <row r="39" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A39" s="2"/>
     </row>
-    <row r="40" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A40" s="2"/>
     </row>
-    <row r="41" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A41" s="2"/>
     </row>
-    <row r="42" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A42" s="2"/>
     </row>
-    <row r="43" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A43" s="2"/>
     </row>
-    <row r="44" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A44" s="2"/>
     </row>
-    <row r="45" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A45" s="2"/>
     </row>
-    <row r="46" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A46" s="2"/>
     </row>
-    <row r="47" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A47" s="2"/>
     </row>
-    <row r="48" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A48" s="2"/>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A49" s="2"/>
     </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A50" s="2"/>
     </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A51" s="2"/>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A52" s="2"/>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" s="2"/>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" s="2"/>
     </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A55" s="2"/>
     </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A56" s="2"/>
     </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A57" s="2"/>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" s="2"/>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" s="2"/>
     </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A60" s="2"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A61" s="2"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A62" s="2"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A63" s="2"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A64" s="2"/>
     </row>
-    <row r="65" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A65" s="2"/>
     </row>
-    <row r="66" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A66" s="2"/>
     </row>
-    <row r="67" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="67" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A67" s="2"/>
     </row>
-    <row r="68" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="68" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A68" s="2"/>
     </row>
-    <row r="69" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="69" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A69" s="2"/>
     </row>
-    <row r="70" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="70" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A70" s="2"/>
     </row>
-    <row r="71" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="71" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A71" s="2"/>
     </row>
-    <row r="72" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="72" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A72" s="2"/>
     </row>
-    <row r="73" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="73" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A73" s="2"/>
     </row>
-    <row r="74" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="74" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A74" s="2"/>
     </row>
-    <row r="75" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="75" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A75" s="2"/>
     </row>
-    <row r="76" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="76" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A76" s="2"/>
     </row>
-    <row r="77" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="77" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A77" s="2"/>
     </row>
-    <row r="78" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="78" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A78" s="2"/>
     </row>
-    <row r="79" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="79" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A79" s="2"/>
     </row>
-    <row r="80" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="80" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A80" s="2"/>
     </row>
-    <row r="81" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="81" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A81" s="2"/>
     </row>
-    <row r="82" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="82" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A82" s="2"/>
     </row>
-    <row r="83" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="83" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A83" s="2"/>
     </row>
-    <row r="84" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="84" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A84" s="2"/>
     </row>
-    <row r="85" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="85" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A85" s="2"/>
     </row>
-    <row r="86" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="86" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A86" s="2"/>
     </row>
-    <row r="87" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="87" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A87" s="2"/>
     </row>
-    <row r="88" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="88" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A88" s="2"/>
     </row>
-    <row r="89" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="89" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A89" s="2"/>
     </row>
-    <row r="90" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="90" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A90" s="2"/>
     </row>
-    <row r="91" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="91" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A91" s="2"/>
     </row>
-    <row r="92" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="92" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A92" s="2"/>
     </row>
-    <row r="93" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="93" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A93" s="2"/>
     </row>
-    <row r="94" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="94" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A94" s="2"/>
     </row>
-    <row r="95" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="95" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A95" s="2"/>
     </row>
-    <row r="96" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="96" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A96" s="2"/>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="97" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A97" s="2"/>
     </row>
-    <row r="98" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="98" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A98" s="2"/>
     </row>
-    <row r="99" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="99" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A99" s="2"/>
     </row>
-    <row r="100" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="100" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A100" s="2"/>
     </row>
-    <row r="101" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="101" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A101" s="2"/>
     </row>
-    <row r="102" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="102" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A102" s="2"/>
     </row>
-    <row r="103" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="103" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A103" s="2"/>
     </row>
-    <row r="104" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="104" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A104" s="2"/>
     </row>
-    <row r="105" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="105" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A105" s="2"/>
     </row>
-    <row r="106" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="106" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A106" s="2"/>
     </row>
-    <row r="107" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="107" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A107" s="2"/>
     </row>
-    <row r="108" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="108" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A108" s="2"/>
     </row>
-    <row r="109" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="109" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A109" s="2"/>
     </row>
-    <row r="110" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="110" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A110" s="2"/>
     </row>
-    <row r="111" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="111" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A111" s="2"/>
     </row>
-    <row r="112" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="112" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A112" s="2"/>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="113" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A113" s="2"/>
     </row>
-    <row r="114" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="114" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A114" s="2"/>
     </row>
-    <row r="115" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="115" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A115" s="2"/>
     </row>
-    <row r="116" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="116" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A116" s="2"/>
     </row>
-    <row r="117" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="117" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A117" s="2"/>
     </row>
-    <row r="118" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="118" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A118" s="2"/>
     </row>
-    <row r="119" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="119" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A119" s="2"/>
     </row>
-    <row r="120" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="120" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A120" s="2"/>
     </row>
-    <row r="121" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="121" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A121" s="2"/>
     </row>
-    <row r="122" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="122" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A122" s="2"/>
     </row>
-    <row r="123" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="123" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A123" s="2"/>
     </row>
-    <row r="124" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="124" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A124" s="2"/>
     </row>
-    <row r="125" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="125" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A125" s="2"/>
     </row>
-    <row r="126" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="126" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A126" s="2"/>
     </row>
-    <row r="127" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="127" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A127" s="2"/>
     </row>
-    <row r="128" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="128" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A128" s="2"/>
     </row>
-    <row r="129" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="129" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A129" s="2"/>
     </row>
-    <row r="130" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="130" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A130" s="2"/>
     </row>
-    <row r="131" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="131" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A131" s="2"/>
     </row>
-    <row r="132" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="132" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A132" s="2"/>
     </row>
-    <row r="133" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="133" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A133" s="2"/>
     </row>
-    <row r="134" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="134" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A134" s="2"/>
     </row>
-    <row r="135" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="135" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A135" s="2"/>
     </row>
-    <row r="136" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="136" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A136" s="2"/>
     </row>
-    <row r="137" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="137" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A137" s="2"/>
     </row>
-    <row r="138" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="138" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A138" s="2"/>
     </row>
-    <row r="139" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="139" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A139" s="2"/>
     </row>
-    <row r="140" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="140" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A140" s="2"/>
     </row>
-    <row r="141" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="141" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A141" s="2"/>
     </row>
-    <row r="142" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="142" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A142" s="2"/>
     </row>
-    <row r="143" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="143" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A143" s="2"/>
     </row>
-    <row r="144" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="144" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A144" s="2"/>
     </row>
-    <row r="145" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="145" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A145" s="2"/>
     </row>
-    <row r="146" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="146" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A146" s="2"/>
     </row>
-    <row r="147" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="147" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A147" s="2"/>
     </row>
-    <row r="148" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="148" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A148" s="2"/>
     </row>
-    <row r="149" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="149" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A149" s="2"/>
     </row>
-    <row r="150" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="150" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A150" s="2"/>
     </row>
-    <row r="151" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="151" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A151" s="2"/>
     </row>
-    <row r="152" spans="1:1" x14ac:dyDescent="0.4">
+    <row r="152" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A152" s="2"/>
     </row>
   </sheetData>
@@ -2633,40 +2646,44 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EC0E44B5-EAEB-4CAD-8DD9-B7C8694AEA97}">
-  <dimension ref="A1:F75"/>
+  <dimension ref="A1:G75"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="L9" sqref="L9"/>
+      <selection pane="bottomLeft" activeCell="C29" sqref="C29"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.6" x14ac:dyDescent="0.4"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="6.765625" style="8" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="11.23046875" style="6" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.140625" style="8" customWidth="1"/>
+    <col min="2" max="2" width="11.28515625" style="6" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.28515625" style="6" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" s="4" customFormat="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:7" s="4" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A1" s="7" t="s">
         <v>14</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>13</v>
       </c>
-      <c r="C1" s="4" t="s">
+      <c r="C1" s="5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="D1" s="4" t="s">
+      <c r="E1" s="4" t="s">
         <v>5</v>
       </c>
-      <c r="E1" s="4" t="s">
+      <c r="F1" s="4" t="s">
         <v>10</v>
       </c>
-      <c r="F1" s="4" t="s">
+      <c r="G1" s="4" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="8" t="s">
         <v>15</v>
       </c>
@@ -2674,19 +2691,22 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="C2">
+        <v>0</v>
+      </c>
+      <c r="D2">
         <v>22.4</v>
       </c>
-      <c r="D2">
+      <c r="E2">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E2">
+      <c r="F2">
         <v>86.7</v>
       </c>
-      <c r="F2">
+      <c r="G2">
         <v>0.86099999999999999</v>
       </c>
     </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="8" t="s">
         <v>15</v>
       </c>
@@ -2694,19 +2714,23 @@
         <v>0.30208333333333331</v>
       </c>
       <c r="C3">
+        <f>C2+(1*15/60)</f>
+        <v>0.25</v>
+      </c>
+      <c r="D3">
         <v>22.3</v>
       </c>
-      <c r="D3">
+      <c r="E3">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="E3">
+      <c r="F3">
         <v>86.7</v>
       </c>
-      <c r="F3">
+      <c r="G3">
         <v>0.86499999999999999</v>
       </c>
     </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="8" t="s">
         <v>15</v>
       </c>
@@ -2714,19 +2738,23 @@
         <v>0.3125</v>
       </c>
       <c r="C4">
+        <f>C3+(1*15/60)</f>
+        <v>0.5</v>
+      </c>
+      <c r="D4">
         <v>22.3</v>
       </c>
-      <c r="D4">
+      <c r="E4">
         <v>5.8000000000000003E-2</v>
       </c>
-      <c r="E4">
+      <c r="F4">
         <v>86.8</v>
       </c>
-      <c r="F4">
+      <c r="G4">
         <v>0.91200000000000003</v>
       </c>
     </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="8" t="s">
         <v>15</v>
       </c>
@@ -2734,19 +2762,23 @@
         <v>0.32291666666666702</v>
       </c>
       <c r="C5">
+        <f>C4+(1*15/60)</f>
+        <v>0.75</v>
+      </c>
+      <c r="D5">
         <v>22.3</v>
       </c>
-      <c r="D5">
+      <c r="E5">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E5">
+      <c r="F5">
         <v>86.9</v>
       </c>
-      <c r="F5">
+      <c r="G5">
         <v>0.83799999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="8" t="s">
         <v>15</v>
       </c>
@@ -2754,19 +2786,23 @@
         <v>0.33333333333333298</v>
       </c>
       <c r="C6">
+        <f>C5+(1*15/60)</f>
+        <v>1</v>
+      </c>
+      <c r="D6">
         <v>22.3</v>
       </c>
-      <c r="D6">
+      <c r="E6">
         <v>4.8000000000000001E-2</v>
       </c>
-      <c r="E6">
+      <c r="F6">
         <v>86.9</v>
       </c>
-      <c r="F6">
+      <c r="G6">
         <v>0.86399999999999999</v>
       </c>
     </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="8" t="s">
         <v>15</v>
       </c>
@@ -2774,19 +2810,23 @@
         <v>0.34375</v>
       </c>
       <c r="C7">
+        <f t="shared" ref="C7:C29" si="0">C6+(1*15/60)</f>
+        <v>1.25</v>
+      </c>
+      <c r="D7">
         <v>30.1</v>
       </c>
-      <c r="D7">
+      <c r="E7">
         <v>1.5669999999999999</v>
       </c>
-      <c r="E7">
+      <c r="F7">
         <v>78.3</v>
       </c>
-      <c r="F7">
+      <c r="G7">
         <v>3.403</v>
       </c>
     </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="8" t="s">
         <v>15</v>
       </c>
@@ -2794,19 +2834,23 @@
         <v>0.35416666666666602</v>
       </c>
       <c r="C8">
+        <f t="shared" si="0"/>
+        <v>1.5</v>
+      </c>
+      <c r="D8">
         <v>47.5</v>
       </c>
-      <c r="D8">
+      <c r="E8">
         <v>0.90800000000000003</v>
       </c>
-      <c r="E8">
+      <c r="F8">
         <v>40.1</v>
       </c>
-      <c r="F8">
+      <c r="G8">
         <v>1.9139999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="8" t="s">
         <v>15</v>
       </c>
@@ -2814,19 +2858,23 @@
         <v>0.36458333333333298</v>
       </c>
       <c r="C9">
+        <f t="shared" si="0"/>
+        <v>1.75</v>
+      </c>
+      <c r="D9">
         <v>46.8</v>
       </c>
-      <c r="D9">
+      <c r="E9">
         <v>1.2669999999999999</v>
       </c>
-      <c r="E9">
+      <c r="F9">
         <v>31.7</v>
       </c>
-      <c r="F9">
+      <c r="G9">
         <v>1.7090000000000001</v>
       </c>
     </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="8" t="s">
         <v>15</v>
       </c>
@@ -2834,19 +2882,23 @@
         <v>0.375</v>
       </c>
       <c r="C10">
+        <f t="shared" si="0"/>
+        <v>2</v>
+      </c>
+      <c r="D10">
         <v>43.5</v>
       </c>
-      <c r="D10">
+      <c r="E10">
         <v>1.7649999999999999</v>
       </c>
-      <c r="E10">
+      <c r="F10">
         <v>41.7</v>
       </c>
-      <c r="F10">
+      <c r="G10">
         <v>2.871</v>
       </c>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="8" t="s">
         <v>15</v>
       </c>
@@ -2854,19 +2906,23 @@
         <v>0.38541666666666602</v>
       </c>
       <c r="C11">
+        <f t="shared" si="0"/>
+        <v>2.25</v>
+      </c>
+      <c r="D11">
         <v>44.6</v>
       </c>
-      <c r="D11">
+      <c r="E11">
         <v>1.599</v>
       </c>
-      <c r="E11">
+      <c r="F11">
         <v>35.5</v>
       </c>
-      <c r="F11">
+      <c r="G11">
         <v>1.3859999999999999</v>
       </c>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="8" t="s">
         <v>15</v>
       </c>
@@ -2874,19 +2930,23 @@
         <v>0.39583333333333298</v>
       </c>
       <c r="C12">
+        <f t="shared" si="0"/>
+        <v>2.5</v>
+      </c>
+      <c r="D12">
         <v>45.6</v>
       </c>
-      <c r="D12">
+      <c r="E12">
         <v>1.5780000000000001</v>
       </c>
-      <c r="E12">
+      <c r="F12">
         <v>33.1</v>
       </c>
-      <c r="F12">
+      <c r="G12">
         <v>1.1930000000000001</v>
       </c>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="8" t="s">
         <v>15</v>
       </c>
@@ -2894,19 +2954,23 @@
         <v>0.40625</v>
       </c>
       <c r="C13">
+        <f t="shared" si="0"/>
+        <v>2.75</v>
+      </c>
+      <c r="D13">
         <v>46.6</v>
       </c>
-      <c r="D13">
+      <c r="E13">
         <v>2.3929999999999998</v>
       </c>
-      <c r="E13">
+      <c r="F13">
         <v>31.3</v>
       </c>
-      <c r="F13">
+      <c r="G13">
         <v>1.7729999999999999</v>
       </c>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="8" t="s">
         <v>15</v>
       </c>
@@ -2914,19 +2978,23 @@
         <v>0.41666666666666702</v>
       </c>
       <c r="C14">
+        <f t="shared" si="0"/>
+        <v>3</v>
+      </c>
+      <c r="D14">
         <v>45.9</v>
       </c>
-      <c r="D14">
+      <c r="E14">
         <v>2.5209999999999999</v>
       </c>
-      <c r="E14">
+      <c r="F14">
         <v>29.4</v>
       </c>
-      <c r="F14">
+      <c r="G14">
         <v>1.986</v>
       </c>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="8" t="s">
         <v>15</v>
       </c>
@@ -2934,19 +3002,23 @@
         <v>0.42708333333333298</v>
       </c>
       <c r="C15">
+        <f t="shared" si="0"/>
+        <v>3.25</v>
+      </c>
+      <c r="D15">
         <v>45.8</v>
       </c>
-      <c r="D15">
+      <c r="E15">
         <v>2.3159999999999998</v>
       </c>
-      <c r="E15">
+      <c r="F15">
         <v>31.1</v>
       </c>
-      <c r="F15">
+      <c r="G15">
         <v>2.8940000000000001</v>
       </c>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="8" t="s">
         <v>15</v>
       </c>
@@ -2954,19 +3026,23 @@
         <v>0.4375</v>
       </c>
       <c r="C16">
+        <f t="shared" si="0"/>
+        <v>3.5</v>
+      </c>
+      <c r="D16">
         <v>41.8</v>
       </c>
-      <c r="D16">
+      <c r="E16">
         <v>0.47</v>
       </c>
-      <c r="E16">
+      <c r="F16">
         <v>34.5</v>
       </c>
-      <c r="F16">
+      <c r="G16">
         <v>4.7329999999999997</v>
       </c>
     </row>
-    <row r="17" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="8" t="s">
         <v>15</v>
       </c>
@@ -2974,19 +3050,23 @@
         <v>0.44791666666666602</v>
       </c>
       <c r="C17">
+        <f t="shared" si="0"/>
+        <v>3.75</v>
+      </c>
+      <c r="D17">
         <v>43.1</v>
       </c>
-      <c r="D17">
+      <c r="E17">
         <v>1.587</v>
       </c>
-      <c r="E17">
+      <c r="F17">
         <v>35.5</v>
       </c>
-      <c r="F17">
+      <c r="G17">
         <v>4.8719999999999999</v>
       </c>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="8" t="s">
         <v>15</v>
       </c>
@@ -2994,19 +3074,23 @@
         <v>0.45833333333333298</v>
       </c>
       <c r="C18">
+        <f t="shared" si="0"/>
+        <v>4</v>
+      </c>
+      <c r="D18">
         <v>44</v>
       </c>
-      <c r="D18">
+      <c r="E18">
         <v>1.75</v>
       </c>
-      <c r="E18">
+      <c r="F18">
         <v>35.9</v>
       </c>
-      <c r="F18">
+      <c r="G18">
         <v>5.1100000000000003</v>
       </c>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="8" t="s">
         <v>15</v>
       </c>
@@ -3014,19 +3098,23 @@
         <v>0.46875</v>
       </c>
       <c r="C19">
+        <f t="shared" si="0"/>
+        <v>4.25</v>
+      </c>
+      <c r="D19">
         <v>43.5</v>
       </c>
-      <c r="D19">
+      <c r="E19">
         <v>0.97599999999999998</v>
       </c>
-      <c r="E19">
+      <c r="F19">
         <v>36.299999999999997</v>
       </c>
-      <c r="F19">
+      <c r="G19">
         <v>5.64</v>
       </c>
     </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="8" t="s">
         <v>15</v>
       </c>
@@ -3034,19 +3122,23 @@
         <v>0.47916666666666602</v>
       </c>
       <c r="C20">
+        <f t="shared" si="0"/>
+        <v>4.5</v>
+      </c>
+      <c r="D20">
         <v>44.4</v>
       </c>
-      <c r="D20">
+      <c r="E20">
         <v>0.95899999999999996</v>
       </c>
-      <c r="E20">
+      <c r="F20">
         <v>37.200000000000003</v>
       </c>
-      <c r="F20">
+      <c r="G20">
         <v>5.1369999999999996</v>
       </c>
     </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="8" t="s">
         <v>15</v>
       </c>
@@ -3054,19 +3146,23 @@
         <v>0.48958333333333298</v>
       </c>
       <c r="C21">
+        <f t="shared" si="0"/>
+        <v>4.75</v>
+      </c>
+      <c r="D21">
         <v>44.6</v>
       </c>
-      <c r="D21">
+      <c r="E21">
         <v>0.72399999999999998</v>
       </c>
-      <c r="E21">
+      <c r="F21">
         <v>36.700000000000003</v>
       </c>
-      <c r="F21">
+      <c r="G21">
         <v>5.2030000000000003</v>
       </c>
     </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="8" t="s">
         <v>15</v>
       </c>
@@ -3074,19 +3170,23 @@
         <v>0.5</v>
       </c>
       <c r="C22">
+        <f t="shared" si="0"/>
+        <v>5</v>
+      </c>
+      <c r="D22">
         <v>44.2</v>
       </c>
-      <c r="D22">
+      <c r="E22">
         <v>1.109</v>
       </c>
-      <c r="E22">
+      <c r="F22">
         <v>31.8</v>
       </c>
-      <c r="F22">
+      <c r="G22">
         <v>4.907</v>
       </c>
     </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="8" t="s">
         <v>15</v>
       </c>
@@ -3094,19 +3194,23 @@
         <v>0.51041666666666596</v>
       </c>
       <c r="C23">
+        <f t="shared" si="0"/>
+        <v>5.25</v>
+      </c>
+      <c r="D23">
         <v>47.5</v>
       </c>
-      <c r="D23">
+      <c r="E23">
         <v>2.403</v>
       </c>
-      <c r="E23">
+      <c r="F23">
         <v>27.1</v>
       </c>
-      <c r="F23">
+      <c r="G23">
         <v>2.2930000000000001</v>
       </c>
     </row>
-    <row r="24" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="8" t="s">
         <v>15</v>
       </c>
@@ -3114,19 +3218,23 @@
         <v>0.52083333333333304</v>
       </c>
       <c r="C24">
+        <f t="shared" si="0"/>
+        <v>5.5</v>
+      </c>
+      <c r="D24">
         <v>44.4</v>
       </c>
-      <c r="D24">
+      <c r="E24">
         <v>1.37</v>
       </c>
-      <c r="E24">
+      <c r="F24">
         <v>28</v>
       </c>
-      <c r="F24">
+      <c r="G24">
         <v>2.512</v>
       </c>
     </row>
-    <row r="25" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="8" t="s">
         <v>15</v>
       </c>
@@ -3134,19 +3242,23 @@
         <v>0.531249999999999</v>
       </c>
       <c r="C25">
+        <f t="shared" si="0"/>
+        <v>5.75</v>
+      </c>
+      <c r="D25">
         <v>37.700000000000003</v>
       </c>
-      <c r="D25">
+      <c r="E25">
         <v>0.71699999999999997</v>
       </c>
-      <c r="E25">
+      <c r="F25">
         <v>37.200000000000003</v>
       </c>
-      <c r="F25">
+      <c r="G25">
         <v>2.8849999999999998</v>
       </c>
     </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="8" t="s">
         <v>15</v>
       </c>
@@ -3154,19 +3266,23 @@
         <v>0.54166666666666596</v>
       </c>
       <c r="C26">
+        <f t="shared" si="0"/>
+        <v>6</v>
+      </c>
+      <c r="D26">
         <v>33.9</v>
       </c>
-      <c r="D26">
+      <c r="E26">
         <v>0.77400000000000002</v>
       </c>
-      <c r="E26">
+      <c r="F26">
         <v>43.4</v>
       </c>
-      <c r="F26">
+      <c r="G26">
         <v>3.843</v>
       </c>
     </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="8" t="s">
         <v>15</v>
       </c>
@@ -3174,19 +3290,23 @@
         <v>0.55208333333333304</v>
       </c>
       <c r="C27">
+        <f t="shared" si="0"/>
+        <v>6.25</v>
+      </c>
+      <c r="D27">
         <v>30.7</v>
       </c>
-      <c r="D27">
+      <c r="E27">
         <v>0.82599999999999996</v>
       </c>
-      <c r="E27">
+      <c r="F27">
         <v>49.1</v>
       </c>
-      <c r="F27">
+      <c r="G27">
         <v>4.4640000000000004</v>
       </c>
     </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="8" t="s">
         <v>15</v>
       </c>
@@ -3194,19 +3314,23 @@
         <v>0.562499999999999</v>
       </c>
       <c r="C28">
+        <f t="shared" si="0"/>
+        <v>6.5</v>
+      </c>
+      <c r="D28">
         <v>31.5</v>
       </c>
-      <c r="D28">
+      <c r="E28">
         <v>0.80700000000000005</v>
       </c>
-      <c r="E28">
+      <c r="F28">
         <v>47.1</v>
       </c>
-      <c r="F28">
+      <c r="G28">
         <v>3.944</v>
       </c>
     </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="8" t="s">
         <v>15</v>
       </c>
@@ -3214,19 +3338,23 @@
         <v>0.57291666666666596</v>
       </c>
       <c r="C29">
+        <f t="shared" si="0"/>
+        <v>6.75</v>
+      </c>
+      <c r="D29">
         <v>27.8</v>
       </c>
-      <c r="D29">
+      <c r="E29">
         <v>0.70599999999999996</v>
       </c>
-      <c r="E29">
+      <c r="F29">
         <v>55.4</v>
       </c>
-      <c r="F29">
+      <c r="G29">
         <v>4.0149999999999997</v>
       </c>
     </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="8" t="s">
         <v>16</v>
       </c>
@@ -3234,13 +3362,16 @@
         <v>0.29166666666666669</v>
       </c>
       <c r="C30">
+        <v>0</v>
+      </c>
+      <c r="D30">
         <v>21.4</v>
       </c>
-      <c r="D30">
+      <c r="E30">
         <v>0.66900000000000004</v>
       </c>
     </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="8" t="s">
         <v>16</v>
       </c>
@@ -3248,13 +3379,17 @@
         <v>0.2986111111111111</v>
       </c>
       <c r="C31">
+        <f>C30+(1*10/60)</f>
+        <v>0.16666666666666666</v>
+      </c>
+      <c r="D31">
         <v>20.7</v>
       </c>
-      <c r="D31">
+      <c r="E31">
         <v>0.7</v>
       </c>
     </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.4">
+    <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="8" t="s">
         <v>16</v>
       </c>
@@ -3262,13 +3397,17 @@
         <v>0.34027777777777773</v>
       </c>
       <c r="C32">
+        <f>C31+1+(1*10/60)</f>
+        <v>1.3333333333333335</v>
+      </c>
+      <c r="D32">
         <v>27.6</v>
       </c>
-      <c r="D32">
+      <c r="E32">
         <v>1.458</v>
       </c>
     </row>
-    <row r="33" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A33" s="8" t="s">
         <v>16</v>
       </c>
@@ -3276,13 +3415,17 @@
         <v>0.34722222222222227</v>
       </c>
       <c r="C33">
+        <f t="shared" ref="C32:C65" si="1">C32+(1*10/60)</f>
+        <v>1.5000000000000002</v>
+      </c>
+      <c r="D33">
         <v>27.3</v>
       </c>
-      <c r="D33">
+      <c r="E33">
         <v>3.76</v>
       </c>
     </row>
-    <row r="34" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A34" s="8" t="s">
         <v>16</v>
       </c>
@@ -3290,13 +3433,17 @@
         <v>0.35416666666666702</v>
       </c>
       <c r="C34">
+        <f t="shared" si="1"/>
+        <v>1.666666666666667</v>
+      </c>
+      <c r="D34">
         <v>35.799999999999997</v>
       </c>
-      <c r="D34">
+      <c r="E34">
         <v>3.1619999999999999</v>
       </c>
     </row>
-    <row r="35" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A35" s="8" t="s">
         <v>16</v>
       </c>
@@ -3304,13 +3451,17 @@
         <v>0.36111111111111099</v>
       </c>
       <c r="C35">
+        <f t="shared" si="1"/>
+        <v>1.8333333333333337</v>
+      </c>
+      <c r="D35">
         <v>32.299999999999997</v>
       </c>
-      <c r="D35">
+      <c r="E35">
         <v>3.2989999999999999</v>
       </c>
     </row>
-    <row r="36" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A36" s="8" t="s">
         <v>16</v>
       </c>
@@ -3318,13 +3469,17 @@
         <v>0.36805555555555602</v>
       </c>
       <c r="C36">
+        <f t="shared" si="1"/>
+        <v>2.0000000000000004</v>
+      </c>
+      <c r="D36">
         <v>33.799999999999997</v>
       </c>
-      <c r="D36">
+      <c r="E36">
         <v>2.5299999999999998</v>
       </c>
     </row>
-    <row r="37" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A37" s="8" t="s">
         <v>16</v>
       </c>
@@ -3332,13 +3487,17 @@
         <v>0.375</v>
       </c>
       <c r="C37">
+        <f t="shared" si="1"/>
+        <v>2.166666666666667</v>
+      </c>
+      <c r="D37">
         <v>35.5</v>
       </c>
-      <c r="D37">
+      <c r="E37">
         <v>2.0569999999999999</v>
       </c>
     </row>
-    <row r="38" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A38" s="8" t="s">
         <v>16</v>
       </c>
@@ -3346,13 +3505,17 @@
         <v>0.38194444444444497</v>
       </c>
       <c r="C38">
+        <f t="shared" si="1"/>
+        <v>2.3333333333333335</v>
+      </c>
+      <c r="D38">
         <v>36.9</v>
       </c>
-      <c r="D38">
+      <c r="E38">
         <v>3.2080000000000002</v>
       </c>
     </row>
-    <row r="39" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A39" s="8" t="s">
         <v>16</v>
       </c>
@@ -3360,13 +3523,17 @@
         <v>0.38888888888888901</v>
       </c>
       <c r="C39">
+        <f t="shared" si="1"/>
+        <v>2.5</v>
+      </c>
+      <c r="D39">
         <v>35.4</v>
       </c>
-      <c r="D39">
+      <c r="E39">
         <v>3.4689999999999999</v>
       </c>
     </row>
-    <row r="40" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A40" s="8" t="s">
         <v>16</v>
       </c>
@@ -3374,13 +3541,17 @@
         <v>0.39583333333333398</v>
       </c>
       <c r="C40">
+        <f t="shared" si="1"/>
+        <v>2.6666666666666665</v>
+      </c>
+      <c r="D40">
         <v>34</v>
       </c>
-      <c r="D40">
+      <c r="E40">
         <v>2.5830000000000002</v>
       </c>
     </row>
-    <row r="41" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A41" s="8" t="s">
         <v>16</v>
       </c>
@@ -3388,13 +3559,17 @@
         <v>0.40277777777777901</v>
       </c>
       <c r="C41">
+        <f t="shared" si="1"/>
+        <v>2.833333333333333</v>
+      </c>
+      <c r="D41">
         <v>31.7</v>
       </c>
-      <c r="D41">
+      <c r="E41">
         <v>2.8279999999999998</v>
       </c>
     </row>
-    <row r="42" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A42" s="8" t="s">
         <v>16</v>
       </c>
@@ -3402,13 +3577,17 @@
         <v>0.40972222222222299</v>
       </c>
       <c r="C42">
+        <f t="shared" si="1"/>
+        <v>2.9999999999999996</v>
+      </c>
+      <c r="D42">
         <v>32.1</v>
       </c>
-      <c r="D42">
+      <c r="E42">
         <v>2.8530000000000002</v>
       </c>
     </row>
-    <row r="43" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A43" s="8" t="s">
         <v>16</v>
       </c>
@@ -3416,13 +3595,17 @@
         <v>0.41666666666666802</v>
       </c>
       <c r="C43">
+        <f t="shared" si="1"/>
+        <v>3.1666666666666661</v>
+      </c>
+      <c r="D43">
         <v>33.4</v>
       </c>
-      <c r="D43">
+      <c r="E43">
         <v>2.5270000000000001</v>
       </c>
     </row>
-    <row r="44" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="44" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A44" s="8" t="s">
         <v>16</v>
       </c>
@@ -3430,13 +3613,17 @@
         <v>0.42361111111111199</v>
       </c>
       <c r="C44">
+        <f t="shared" si="1"/>
+        <v>3.3333333333333326</v>
+      </c>
+      <c r="D44">
         <v>36.200000000000003</v>
       </c>
-      <c r="D44">
+      <c r="E44">
         <v>2.431</v>
       </c>
     </row>
-    <row r="45" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="45" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A45" s="8" t="s">
         <v>16</v>
       </c>
@@ -3444,13 +3631,17 @@
         <v>0.43055555555555702</v>
       </c>
       <c r="C45">
+        <f t="shared" si="1"/>
+        <v>3.4999999999999991</v>
+      </c>
+      <c r="D45">
         <v>35.700000000000003</v>
       </c>
-      <c r="D45">
+      <c r="E45">
         <v>2.5870000000000002</v>
       </c>
     </row>
-    <row r="46" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="46" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A46" s="8" t="s">
         <v>16</v>
       </c>
@@ -3458,13 +3649,17 @@
         <v>0.437500000000001</v>
       </c>
       <c r="C46">
+        <f t="shared" si="1"/>
+        <v>3.6666666666666656</v>
+      </c>
+      <c r="D46">
         <v>32.4</v>
       </c>
-      <c r="D46">
+      <c r="E46">
         <v>3.198</v>
       </c>
     </row>
-    <row r="47" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="47" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A47" s="8" t="s">
         <v>16</v>
       </c>
@@ -3472,13 +3667,17 @@
         <v>0.44444444444444597</v>
       </c>
       <c r="C47">
+        <f t="shared" si="1"/>
+        <v>3.8333333333333321</v>
+      </c>
+      <c r="D47">
         <v>34.5</v>
       </c>
-      <c r="D47">
+      <c r="E47">
         <v>2.8370000000000002</v>
       </c>
     </row>
-    <row r="48" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="48" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A48" s="8" t="s">
         <v>16</v>
       </c>
@@ -3486,13 +3685,17 @@
         <v>0.45138888888889001</v>
       </c>
       <c r="C48">
+        <f t="shared" si="1"/>
+        <v>3.9999999999999987</v>
+      </c>
+      <c r="D48">
         <v>34.299999999999997</v>
       </c>
-      <c r="D48">
+      <c r="E48">
         <v>2.52</v>
       </c>
     </row>
-    <row r="49" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="49" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A49" s="8" t="s">
         <v>16</v>
       </c>
@@ -3500,13 +3703,17 @@
         <v>0.45833333333333498</v>
       </c>
       <c r="C49">
+        <f t="shared" si="1"/>
+        <v>4.1666666666666652</v>
+      </c>
+      <c r="D49">
         <v>35.4</v>
       </c>
-      <c r="D49">
+      <c r="E49">
         <v>2.4510000000000001</v>
       </c>
     </row>
-    <row r="50" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="50" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A50" s="8" t="s">
         <v>16</v>
       </c>
@@ -3514,13 +3721,17 @@
         <v>0.46527777777778001</v>
       </c>
       <c r="C50">
+        <f t="shared" si="1"/>
+        <v>4.3333333333333321</v>
+      </c>
+      <c r="D50">
         <v>36.299999999999997</v>
       </c>
-      <c r="D50">
+      <c r="E50">
         <v>2.5779999999999998</v>
       </c>
     </row>
-    <row r="51" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="51" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A51" s="8" t="s">
         <v>16</v>
       </c>
@@ -3528,13 +3739,17 @@
         <v>0.47222222222222399</v>
       </c>
       <c r="C51">
+        <f t="shared" si="1"/>
+        <v>4.4999999999999991</v>
+      </c>
+      <c r="D51">
         <v>35.200000000000003</v>
       </c>
-      <c r="D51">
+      <c r="E51">
         <v>2.76</v>
       </c>
     </row>
-    <row r="52" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="52" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A52" s="8" t="s">
         <v>16</v>
       </c>
@@ -3542,13 +3757,17 @@
         <v>0.47916666666666902</v>
       </c>
       <c r="C52">
+        <f t="shared" si="1"/>
+        <v>4.6666666666666661</v>
+      </c>
+      <c r="D52">
         <v>35.5</v>
       </c>
-      <c r="D52">
+      <c r="E52">
         <v>2.1139999999999999</v>
       </c>
     </row>
-    <row r="53" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="53" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A53" s="8" t="s">
         <v>16</v>
       </c>
@@ -3556,13 +3775,17 @@
         <v>0.48611111111111299</v>
       </c>
       <c r="C53">
+        <f t="shared" si="1"/>
+        <v>4.833333333333333</v>
+      </c>
+      <c r="D53">
         <v>34.700000000000003</v>
       </c>
-      <c r="D53">
+      <c r="E53">
         <v>2.9649999999999999</v>
       </c>
     </row>
-    <row r="54" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="54" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A54" s="8" t="s">
         <v>16</v>
       </c>
@@ -3570,13 +3793,17 @@
         <v>0.49305555555555802</v>
       </c>
       <c r="C54">
+        <f t="shared" si="1"/>
+        <v>5</v>
+      </c>
+      <c r="D54">
         <v>34.4</v>
       </c>
-      <c r="D54">
+      <c r="E54">
         <v>2.5680000000000001</v>
       </c>
     </row>
-    <row r="55" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="55" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A55" s="8" t="s">
         <v>16</v>
       </c>
@@ -3584,13 +3811,17 @@
         <v>0.500000000000002</v>
       </c>
       <c r="C55">
+        <f t="shared" si="1"/>
+        <v>5.166666666666667</v>
+      </c>
+      <c r="D55">
         <v>36.5</v>
       </c>
-      <c r="D55">
+      <c r="E55">
         <v>2.2189999999999999</v>
       </c>
     </row>
-    <row r="56" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="56" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A56" s="8" t="s">
         <v>16</v>
       </c>
@@ -3598,13 +3829,17 @@
         <v>0.50694444444444697</v>
       </c>
       <c r="C56">
+        <f t="shared" si="1"/>
+        <v>5.3333333333333339</v>
+      </c>
+      <c r="D56">
         <v>37.6</v>
       </c>
-      <c r="D56">
+      <c r="E56">
         <v>2.1120000000000001</v>
       </c>
     </row>
-    <row r="57" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="57" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A57" s="8" t="s">
         <v>16</v>
       </c>
@@ -3612,13 +3847,17 @@
         <v>0.51388888888889095</v>
       </c>
       <c r="C57">
+        <f t="shared" si="1"/>
+        <v>5.5000000000000009</v>
+      </c>
+      <c r="D57">
         <v>37.200000000000003</v>
       </c>
-      <c r="D57">
+      <c r="E57">
         <v>2.181</v>
       </c>
     </row>
-    <row r="58" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="58" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A58" s="8" t="s">
         <v>16</v>
       </c>
@@ -3626,13 +3865,17 @@
         <v>0.52083333333333603</v>
       </c>
       <c r="C58">
+        <f t="shared" si="1"/>
+        <v>5.6666666666666679</v>
+      </c>
+      <c r="D58">
         <v>36.9</v>
       </c>
-      <c r="D58">
+      <c r="E58">
         <v>2.3090000000000002</v>
       </c>
     </row>
-    <row r="59" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="59" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A59" s="8" t="s">
         <v>16</v>
       </c>
@@ -3640,13 +3883,17 @@
         <v>0.52777777777778001</v>
       </c>
       <c r="C59">
+        <f t="shared" si="1"/>
+        <v>5.8333333333333348</v>
+      </c>
+      <c r="D59">
         <v>37.299999999999997</v>
       </c>
-      <c r="D59">
+      <c r="E59">
         <v>2.1819999999999999</v>
       </c>
     </row>
-    <row r="60" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="60" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A60" s="8" t="s">
         <v>16</v>
       </c>
@@ -3654,13 +3901,17 @@
         <v>0.53472222222222499</v>
       </c>
       <c r="C60">
+        <f t="shared" si="1"/>
+        <v>6.0000000000000018</v>
+      </c>
+      <c r="D60">
         <v>30.9</v>
       </c>
-      <c r="D60">
+      <c r="E60">
         <v>2.2090000000000001</v>
       </c>
     </row>
-    <row r="61" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="61" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A61" s="8" t="s">
         <v>16</v>
       </c>
@@ -3668,13 +3919,17 @@
         <v>0.54166666666666996</v>
       </c>
       <c r="C61">
+        <f t="shared" si="1"/>
+        <v>6.1666666666666687</v>
+      </c>
+      <c r="D61">
         <v>31.4</v>
       </c>
-      <c r="D61">
+      <c r="E61">
         <v>1.3089999999999999</v>
       </c>
     </row>
-    <row r="62" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="62" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A62" s="8" t="s">
         <v>16</v>
       </c>
@@ -3682,13 +3937,17 @@
         <v>0.54861111111111505</v>
       </c>
       <c r="C62">
+        <f t="shared" si="1"/>
+        <v>6.3333333333333357</v>
+      </c>
+      <c r="D62">
         <v>25.6</v>
       </c>
-      <c r="D62">
+      <c r="E62">
         <v>1.5429999999999999</v>
       </c>
     </row>
-    <row r="63" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="63" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A63" s="8" t="s">
         <v>16</v>
       </c>
@@ -3696,13 +3955,17 @@
         <v>0.55555555555556002</v>
       </c>
       <c r="C63">
+        <f t="shared" si="1"/>
+        <v>6.5000000000000027</v>
+      </c>
+      <c r="D63">
         <v>23.7</v>
       </c>
-      <c r="D63">
+      <c r="E63">
         <v>1.7589999999999999</v>
       </c>
     </row>
-    <row r="64" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="64" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A64" s="8" t="s">
         <v>16</v>
       </c>
@@ -3710,13 +3973,17 @@
         <v>0.562500000000005</v>
       </c>
       <c r="C64">
+        <f t="shared" si="1"/>
+        <v>6.6666666666666696</v>
+      </c>
+      <c r="D64">
         <v>21.8</v>
       </c>
-      <c r="D64">
+      <c r="E64">
         <v>1.008</v>
       </c>
     </row>
-    <row r="65" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="65" spans="1:5" x14ac:dyDescent="0.25">
       <c r="A65" s="8" t="s">
         <v>16</v>
       </c>
@@ -3724,41 +3991,55 @@
         <v>0.56944444444444997</v>
       </c>
       <c r="C65">
+        <f t="shared" si="1"/>
+        <v>6.8333333333333366</v>
+      </c>
+      <c r="D65">
         <v>21.4</v>
       </c>
-      <c r="D65">
+      <c r="E65">
         <v>0.89600000000000002</v>
       </c>
     </row>
-    <row r="66" spans="1:4" x14ac:dyDescent="0.4">
+    <row r="66" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B66" s="9"/>
-    </row>
-    <row r="67" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C66" s="9"/>
+    </row>
+    <row r="67" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B67" s="9"/>
-    </row>
-    <row r="68" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C67" s="9"/>
+    </row>
+    <row r="68" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B68" s="9"/>
-    </row>
-    <row r="69" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C68" s="9"/>
+    </row>
+    <row r="69" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B69" s="9"/>
-    </row>
-    <row r="70" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C69" s="9"/>
+    </row>
+    <row r="70" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B70" s="9"/>
-    </row>
-    <row r="71" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C70" s="9"/>
+    </row>
+    <row r="71" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B71" s="9"/>
-    </row>
-    <row r="72" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C71" s="9"/>
+    </row>
+    <row r="72" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B72" s="9"/>
-    </row>
-    <row r="73" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C72" s="9"/>
+    </row>
+    <row r="73" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B73" s="9"/>
-    </row>
-    <row r="74" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C73" s="9"/>
+    </row>
+    <row r="74" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B74" s="9"/>
-    </row>
-    <row r="75" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="C74" s="9"/>
+    </row>
+    <row r="75" spans="1:5" x14ac:dyDescent="0.25">
       <c r="B75" s="9"/>
+      <c r="C75" s="9"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>